<commit_message>
Fix: Rounded query 2 output
</commit_message>
<xml_diff>
--- a/query2-results.xlsx
+++ b/query2-results.xlsx
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>50.84924623115578</v>
+        <v>50.85</v>
       </c>
     </row>
     <row r="3">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>50.51983077736647</v>
+        <v>50.52</v>
       </c>
     </row>
     <row r="4">
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>49.95681511470985</v>
+        <v>49.96</v>
       </c>
     </row>
     <row r="5">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>50.05913272010513</v>
+        <v>50.06</v>
       </c>
     </row>
     <row r="6">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>52.69192634560906</v>
+        <v>52.69</v>
       </c>
     </row>
     <row r="7">
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>50.6330567964263</v>
+        <v>50.63</v>
       </c>
     </row>
     <row r="8">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>48.0912034538586</v>
+        <v>48.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>